<commit_message>
parametros de seguridad listo
</commit_message>
<xml_diff>
--- a/Documentacion/Parametros.xlsx
+++ b/Documentacion/Parametros.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="123">
   <si>
     <t>Cambio de Contraseña</t>
   </si>
@@ -381,6 +381,18 @@
   </si>
   <si>
     <t>(0) Error al Asiganar Opciones</t>
+  </si>
+  <si>
+    <t>Registro Privilegio</t>
+  </si>
+  <si>
+    <t>Codigo Privilegio</t>
+  </si>
+  <si>
+    <t>(1) Privilegio Registrado</t>
+  </si>
+  <si>
+    <t>(0) Error al Registrar Privilegio</t>
   </si>
 </sst>
 </file>
@@ -547,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -610,30 +622,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -646,32 +634,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -685,33 +772,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -742,101 +805,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AM57"/>
+  <dimension ref="B2:AM55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="K7" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,15 +1142,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
       <c r="K2" s="23"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
@@ -1191,38 +1191,38 @@
       <c r="AM3" s="3"/>
     </row>
     <row r="4" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="99" t="s">
+      <c r="C4" s="96"/>
+      <c r="D4" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99" t="s">
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99" t="s">
+      <c r="H4" s="92"/>
+      <c r="I4" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="99"/>
+      <c r="J4" s="92"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57" t="s">
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57" t="s">
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="S4" s="57"/>
+      <c r="S4" s="80"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
@@ -1245,24 +1245,24 @@
       <c r="AM4" s="3"/>
     </row>
     <row r="5" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="100"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="90"/>
-      <c r="Q5" s="90"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
@@ -1285,38 +1285,38 @@
       <c r="AM5" s="3"/>
     </row>
     <row r="6" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="58" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="58" t="s">
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="59"/>
-      <c r="I6" s="58" t="s">
+      <c r="H6" s="40"/>
+      <c r="I6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="59"/>
+      <c r="J6" s="40"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="84" t="s">
+      <c r="M6" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="N6" s="85"/>
-      <c r="O6" s="85"/>
-      <c r="P6" s="84" t="s">
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" s="86"/>
-      <c r="R6" s="44" t="s">
+      <c r="Q6" s="64"/>
+      <c r="R6" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="S6" s="45"/>
+      <c r="S6" s="54"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -1339,30 +1339,30 @@
       <c r="AM6" s="3"/>
     </row>
     <row r="7" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="62" t="s">
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="46"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="87" t="s">
+      <c r="M7" s="62"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="Q7" s="89"/>
-      <c r="R7" s="42" t="s">
+      <c r="Q7" s="65"/>
+      <c r="R7" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="S7" s="43"/>
+      <c r="S7" s="56"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
@@ -1385,36 +1385,36 @@
       <c r="AM7" s="3"/>
     </row>
     <row r="8" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="58" t="s">
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="74"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="58" t="s">
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="59"/>
-      <c r="I8" s="58" t="s">
+      <c r="H8" s="40"/>
+      <c r="I8" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="59"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="84" t="s">
+      <c r="M8" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
-      <c r="P8" s="84" t="s">
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="Q8" s="86"/>
-      <c r="R8" s="44" t="s">
+      <c r="Q8" s="64"/>
+      <c r="R8" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="S8" s="45"/>
+      <c r="S8" s="54"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
@@ -1437,30 +1437,30 @@
       <c r="AM8" s="3"/>
     </row>
     <row r="9" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="55"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="60" t="s">
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="61"/>
+      <c r="J9" s="43"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="88"/>
-      <c r="O9" s="88"/>
-      <c r="P9" s="87" t="s">
+      <c r="M9" s="62"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="Q9" s="89"/>
-      <c r="R9" s="42" t="s">
+      <c r="Q9" s="65"/>
+      <c r="R9" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="S9" s="43"/>
+      <c r="S9" s="56"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
@@ -1483,32 +1483,32 @@
       <c r="AM9" s="3"/>
     </row>
     <row r="10" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="55"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="60" t="s">
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="61"/>
+      <c r="J10" s="43"/>
       <c r="K10" s="24"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="50" t="s">
+      <c r="M10" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="N10" s="44"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="83" t="s">
+      <c r="N10" s="57"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="Q10" s="83"/>
-      <c r="R10" s="50" t="s">
+      <c r="Q10" s="93"/>
+      <c r="R10" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="S10" s="45"/>
+      <c r="S10" s="54"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
@@ -1531,34 +1531,34 @@
       <c r="AM10" s="3"/>
     </row>
     <row r="11" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="58" t="s">
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="58" t="s">
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="58" t="s">
+      <c r="H11" s="40"/>
+      <c r="I11" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="59"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="24"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="82" t="s">
+      <c r="M11" s="51"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="Q11" s="82"/>
-      <c r="R11" s="49" t="s">
+      <c r="Q11" s="94"/>
+      <c r="R11" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="S11" s="43"/>
+      <c r="S11" s="56"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
@@ -1581,34 +1581,34 @@
       <c r="AM11" s="3"/>
     </row>
     <row r="12" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="55"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="55" t="s">
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="56"/>
-      <c r="I12" s="60" t="s">
+      <c r="H12" s="50"/>
+      <c r="I12" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="61"/>
+      <c r="J12" s="43"/>
       <c r="K12" s="24"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="50" t="s">
+      <c r="M12" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="N12" s="44"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="81" t="s">
+      <c r="N12" s="57"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="50" t="s">
+      <c r="Q12" s="99"/>
+      <c r="R12" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="S12" s="45"/>
+      <c r="S12" s="54"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
@@ -1631,30 +1631,30 @@
       <c r="AM12" s="3"/>
     </row>
     <row r="13" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="62" t="s">
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="63"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="46"/>
       <c r="K13" s="24"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="82" t="s">
+      <c r="M13" s="51"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="49" t="s">
+      <c r="Q13" s="94"/>
+      <c r="R13" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="S13" s="43"/>
+      <c r="S13" s="56"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
@@ -1677,36 +1677,36 @@
       <c r="AM13" s="3"/>
     </row>
     <row r="14" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="58" t="s">
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="74"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="58" t="s">
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="59"/>
-      <c r="I14" s="58" t="s">
+      <c r="H14" s="40"/>
+      <c r="I14" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="J14" s="59"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="91" t="s">
+      <c r="J14" s="40"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="N14" s="92"/>
-      <c r="O14" s="93"/>
-      <c r="P14" s="84" t="s">
+      <c r="N14" s="71"/>
+      <c r="O14" s="72"/>
+      <c r="P14" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="Q14" s="86"/>
-      <c r="R14" s="44" t="s">
+      <c r="Q14" s="64"/>
+      <c r="R14" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="S14" s="45"/>
+      <c r="S14" s="54"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
@@ -1729,28 +1729,28 @@
       <c r="AM14" s="3"/>
     </row>
     <row r="15" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="104"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="95"/>
-      <c r="O15" s="96"/>
-      <c r="P15" s="87" t="s">
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="42" t="s">
+      <c r="Q15" s="65"/>
+      <c r="R15" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="S15" s="43"/>
+      <c r="S15" s="56"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
@@ -1773,38 +1773,38 @@
       <c r="AM15" s="3"/>
     </row>
     <row r="16" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="50" t="s">
+      <c r="C16" s="54"/>
+      <c r="D16" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="30" t="s">
+      <c r="E16" s="57"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="36" t="s">
+      <c r="H16" s="54"/>
+      <c r="I16" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="J16" s="31"/>
+      <c r="J16" s="35"/>
       <c r="K16" s="24"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="50" t="s">
+      <c r="M16" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="N16" s="44"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="79" t="s">
+      <c r="N16" s="57"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="Q16" s="80"/>
-      <c r="R16" s="50" t="s">
+      <c r="Q16" s="69"/>
+      <c r="R16" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="S16" s="45"/>
+      <c r="S16" s="54"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
@@ -1827,32 +1827,32 @@
       <c r="AM16" s="3"/>
     </row>
     <row r="17" spans="2:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="49"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="32" t="s">
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="33"/>
-      <c r="I17" s="37" t="s">
+      <c r="H17" s="56"/>
+      <c r="I17" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="J17" s="33"/>
+      <c r="J17" s="34"/>
       <c r="K17" s="24"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="48" t="s">
+      <c r="M17" s="51"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="48" t="s">
+      <c r="Q17" s="52"/>
+      <c r="R17" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="S17" s="47"/>
+      <c r="S17" s="52"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -1875,32 +1875,32 @@
       <c r="AM17" s="3"/>
     </row>
     <row r="18" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="48"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="34" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="35"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="56"/>
       <c r="K18" s="24"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="50" t="s">
+      <c r="M18" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="N18" s="44"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="50" t="s">
+      <c r="N18" s="57"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="50" t="s">
+      <c r="Q18" s="54"/>
+      <c r="R18" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="S18" s="45"/>
+      <c r="S18" s="54"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -1923,19 +1923,30 @@
       <c r="AM18" s="3"/>
     </row>
     <row r="19" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="51"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="100" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="101"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="52"/>
       <c r="K19" s="24"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="48" t="s">
+      <c r="M19" s="51"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="48" t="s">
+      <c r="Q19" s="52"/>
+      <c r="R19" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="S19" s="47"/>
+      <c r="S19" s="52"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
@@ -1958,24 +1969,30 @@
       <c r="AM19" s="3"/>
     </row>
     <row r="20" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="24"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="M20" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
+      <c r="P20" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q20" s="64"/>
+      <c r="R20" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="S20" s="54"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
@@ -1998,24 +2015,28 @@
       <c r="AM20" s="3"/>
     </row>
     <row r="21" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
       <c r="K21" s="4"/>
       <c r="L21" s="26"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q21" s="65"/>
+      <c r="R21" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="S21" s="52"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
@@ -2047,7 +2068,6 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="26"/>
-      <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
@@ -2076,32 +2096,38 @@
       <c r="AM22" s="3"/>
     </row>
     <row r="23" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="57" t="s">
+      <c r="C23" s="77"/>
+      <c r="D23" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57" t="s">
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57" t="s">
+      <c r="H23" s="80"/>
+      <c r="I23" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="57"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="S23" s="80"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -2124,23 +2150,24 @@
       <c r="AM23" s="3"/>
     </row>
     <row r="24" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="53"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
       <c r="K24" s="4"/>
       <c r="L24" s="19"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="80"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="80"/>
+      <c r="S24" s="80"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -2163,15 +2190,15 @@
       <c r="AM24" s="3"/>
     </row>
     <row r="25" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="50" t="s">
+      <c r="C25" s="54"/>
+      <c r="D25" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="44"/>
-      <c r="F25" s="45"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="54"/>
       <c r="G25" s="5" t="s">
         <v>17</v>
       </c>
@@ -2181,19 +2208,19 @@
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="2"/>
-      <c r="M25" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q25" s="57"/>
-      <c r="R25" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="S25" s="57"/>
+      <c r="M25" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="82"/>
+      <c r="O25" s="83"/>
+      <c r="P25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="S25" s="6"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -2216,11 +2243,11 @@
       <c r="AM25" s="3"/>
     </row>
     <row r="26" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="48"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="47"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="7" t="s">
         <v>18</v>
       </c>
@@ -2230,13 +2257,17 @@
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="2"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="57"/>
-      <c r="Q26" s="57"/>
-      <c r="R26" s="57"/>
-      <c r="S26" s="57"/>
+      <c r="M26" s="84"/>
+      <c r="N26" s="85"/>
+      <c r="O26" s="86"/>
+      <c r="P26" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="S26" s="67"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -2259,15 +2290,15 @@
       <c r="AM26" s="3"/>
     </row>
     <row r="27" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="50" t="s">
+      <c r="C27" s="54"/>
+      <c r="D27" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="44"/>
-      <c r="F27" s="45"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="54"/>
       <c r="G27" s="5" t="s">
         <v>17</v>
       </c>
@@ -2277,26 +2308,22 @@
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="25"/>
-      <c r="M27" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="N27" s="65"/>
-      <c r="O27" s="66"/>
-      <c r="P27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="S27" s="6"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="8"/>
     </row>
     <row r="28" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="48"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="47"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="52"/>
       <c r="G28" s="7" t="s">
         <v>18</v>
       </c>
@@ -2306,28 +2333,30 @@
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="25"/>
-      <c r="M28" s="67"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="77" t="s">
-        <v>41</v>
-      </c>
-      <c r="S28" s="78"/>
+      <c r="M28" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="N28" s="82"/>
+      <c r="O28" s="83"/>
+      <c r="P28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S28" s="6"/>
     </row>
     <row r="29" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="50" t="s">
+      <c r="C29" s="54"/>
+      <c r="D29" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="44"/>
-      <c r="F29" s="45"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="54"/>
       <c r="G29" s="10" t="s">
         <v>17</v>
       </c>
@@ -2337,22 +2366,24 @@
       </c>
       <c r="J29" s="14"/>
       <c r="K29" s="25"/>
-      <c r="M29" s="71"/>
-      <c r="N29" s="72"/>
-      <c r="O29" s="73"/>
-      <c r="P29" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="8"/>
+      <c r="M29" s="84"/>
+      <c r="N29" s="85"/>
+      <c r="O29" s="86"/>
+      <c r="P29" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="S29" s="11"/>
     </row>
     <row r="30" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="49"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="43"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="56"/>
       <c r="G30" s="9" t="s">
         <v>25</v>
       </c>
@@ -2362,50 +2393,48 @@
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="25"/>
-      <c r="M30" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="N30" s="65"/>
-      <c r="O30" s="66"/>
-      <c r="P30" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="S30" s="6"/>
+      <c r="M30" s="88"/>
+      <c r="N30" s="89"/>
+      <c r="O30" s="90"/>
+      <c r="P30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="8"/>
     </row>
     <row r="31" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="49"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="43"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H31" s="11"/>
       <c r="J31" s="16"/>
       <c r="K31" s="4"/>
-      <c r="M31" s="67"/>
-      <c r="N31" s="68"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="S31" s="11"/>
+      <c r="M31" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" s="82"/>
+      <c r="O31" s="83"/>
+      <c r="P31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S31" s="6"/>
     </row>
     <row r="32" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="48"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="47"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="12" t="s">
         <v>26</v>
       </c>
@@ -2413,26 +2442,28 @@
       <c r="I32" s="17"/>
       <c r="J32" s="18"/>
       <c r="K32" s="4"/>
-      <c r="M32" s="71"/>
-      <c r="N32" s="72"/>
-      <c r="O32" s="73"/>
-      <c r="P32" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="8"/>
+      <c r="M32" s="84"/>
+      <c r="N32" s="85"/>
+      <c r="O32" s="86"/>
+      <c r="P32" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="S32" s="11"/>
     </row>
     <row r="33" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="50" t="s">
+      <c r="C33" s="54"/>
+      <c r="D33" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="54"/>
       <c r="G33" s="10" t="s">
         <v>17</v>
       </c>
@@ -2442,26 +2473,22 @@
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="4"/>
-      <c r="M33" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="N33" s="65"/>
-      <c r="O33" s="66"/>
-      <c r="P33" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="S33" s="6"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="89"/>
+      <c r="O33" s="90"/>
+      <c r="P33" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="8"/>
     </row>
     <row r="34" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="49"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="21"/>
       <c r="H34" s="11"/>
       <c r="I34" s="28" t="s">
@@ -2469,260 +2496,318 @@
       </c>
       <c r="J34" s="11"/>
       <c r="K34" s="4"/>
-      <c r="M34" s="67"/>
-      <c r="N34" s="68"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="S34" s="11"/>
+      <c r="M34" s="81" t="s">
+        <v>52</v>
+      </c>
+      <c r="N34" s="82"/>
+      <c r="O34" s="83"/>
+      <c r="P34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="S34" s="6"/>
     </row>
     <row r="35" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="48"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="47"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="52"/>
       <c r="G35" s="7"/>
       <c r="H35" s="8"/>
       <c r="I35" s="29" t="s">
         <v>83</v>
       </c>
       <c r="J35" s="8"/>
-      <c r="M35" s="71"/>
-      <c r="N35" s="72"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="8"/>
+      <c r="M35" s="84"/>
+      <c r="N35" s="85"/>
+      <c r="O35" s="86"/>
+      <c r="P35" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="S35" s="11"/>
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M36" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="N36" s="65"/>
-      <c r="O36" s="66"/>
-      <c r="P36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="S36" s="6"/>
+      <c r="M36" s="88"/>
+      <c r="N36" s="89"/>
+      <c r="O36" s="90"/>
+      <c r="P36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="8"/>
     </row>
     <row r="37" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M37" s="67"/>
-      <c r="N37" s="68"/>
-      <c r="O37" s="69"/>
-      <c r="P37" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="S37" s="11"/>
+      <c r="M37" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="N37" s="57"/>
+      <c r="O37" s="54"/>
+      <c r="P37" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="S37" s="6"/>
     </row>
     <row r="38" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M38" s="71"/>
-      <c r="N38" s="72"/>
-      <c r="O38" s="73"/>
-      <c r="P38" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="8"/>
+      <c r="M38" s="55"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="S38" s="11"/>
     </row>
     <row r="39" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M39" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="N39" s="44"/>
-      <c r="O39" s="45"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
       <c r="P39" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="S39" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="11"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M40" s="49"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
+      <c r="M40" s="55"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="56"/>
       <c r="P40" s="9" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="Q40" s="11"/>
-      <c r="R40" s="21" t="s">
-        <v>63</v>
-      </c>
+      <c r="R40" s="21"/>
       <c r="S40" s="11"/>
     </row>
     <row r="41" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M41" s="49"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="42"/>
+      <c r="M41" s="55"/>
+      <c r="N41" s="58"/>
+      <c r="O41" s="56"/>
       <c r="P41" s="9" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="Q41" s="11"/>
-      <c r="R41" s="21"/>
       <c r="S41" s="11"/>
     </row>
     <row r="42" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M42" s="49"/>
-      <c r="N42" s="42"/>
-      <c r="O42" s="43"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="56"/>
       <c r="P42" s="9" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="Q42" s="11"/>
       <c r="R42" s="21"/>
       <c r="S42" s="11"/>
     </row>
     <row r="43" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M43" s="49"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="43"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="56"/>
       <c r="P43" s="9" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="Q43" s="11"/>
+      <c r="R43" s="21"/>
       <c r="S43" s="11"/>
     </row>
     <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M44" s="49"/>
-      <c r="N44" s="42"/>
-      <c r="O44" s="43"/>
+      <c r="M44" s="55"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="56"/>
       <c r="P44" s="9" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="Q44" s="11"/>
       <c r="R44" s="21"/>
       <c r="S44" s="11"/>
     </row>
     <row r="45" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M45" s="49"/>
-      <c r="N45" s="42"/>
-      <c r="O45" s="43"/>
-      <c r="P45" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="21"/>
-      <c r="S45" s="11"/>
+      <c r="M45" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="N45" s="82"/>
+      <c r="O45" s="83"/>
+      <c r="P45" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="S45" s="6"/>
     </row>
     <row r="46" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M46" s="49"/>
-      <c r="N46" s="42"/>
-      <c r="O46" s="43"/>
+      <c r="M46" s="84"/>
+      <c r="N46" s="85"/>
+      <c r="O46" s="86"/>
       <c r="P46" s="9" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="Q46" s="11"/>
-      <c r="R46" s="21"/>
+      <c r="R46" s="21" t="s">
+        <v>66</v>
+      </c>
       <c r="S46" s="11"/>
     </row>
     <row r="47" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M47" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="N47" s="65"/>
-      <c r="O47" s="66"/>
-      <c r="P47" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="S47" s="6"/>
+      <c r="M47" s="84"/>
+      <c r="N47" s="85"/>
+      <c r="O47" s="86"/>
+      <c r="P47" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="S47" s="11"/>
     </row>
     <row r="48" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M48" s="67"/>
-      <c r="N48" s="68"/>
-      <c r="O48" s="69"/>
+      <c r="M48" s="84"/>
+      <c r="N48" s="85"/>
+      <c r="O48" s="86"/>
       <c r="P48" s="9" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="Q48" s="11"/>
       <c r="R48" s="21" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="S48" s="11"/>
     </row>
     <row r="49" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M49" s="67"/>
-      <c r="N49" s="68"/>
-      <c r="O49" s="69"/>
-      <c r="P49" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="S49" s="11"/>
+      <c r="M49" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="N49" s="57"/>
+      <c r="O49" s="54"/>
+      <c r="P49" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="S49" s="6"/>
     </row>
     <row r="50" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M50" s="67"/>
-      <c r="N50" s="68"/>
-      <c r="O50" s="69"/>
-      <c r="P50" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="S50" s="11"/>
-    </row>
-    <row r="51" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M51" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="N51" s="44"/>
-      <c r="O51" s="45"/>
-      <c r="P51" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="S51" s="6"/>
-    </row>
-    <row r="52" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M52" s="48"/>
-      <c r="N52" s="46"/>
-      <c r="O52" s="47"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="8"/>
-      <c r="R52" s="12" t="s">
+      <c r="M50" s="51"/>
+      <c r="N50" s="59"/>
+      <c r="O50" s="52"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="S52" s="8"/>
-    </row>
-    <row r="56" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M56" s="20"/>
-    </row>
-    <row r="57" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M57" s="20"/>
+      <c r="S50" s="8"/>
+    </row>
+    <row r="54" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M54" s="20"/>
+    </row>
+    <row r="55" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M55" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="89">
+  <mergeCells count="98">
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="D16:F19"/>
+    <mergeCell ref="B16:C19"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M6:O7"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P4:Q5"/>
+    <mergeCell ref="R4:S5"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="M49:O50"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="M28:O30"/>
+    <mergeCell ref="M31:O33"/>
+    <mergeCell ref="M34:O36"/>
+    <mergeCell ref="M37:O44"/>
+    <mergeCell ref="M23:O24"/>
+    <mergeCell ref="M25:O27"/>
+    <mergeCell ref="D25:F26"/>
+    <mergeCell ref="D27:F28"/>
+    <mergeCell ref="D29:F32"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M4:O5"/>
+    <mergeCell ref="D23:F24"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="G23:H24"/>
+    <mergeCell ref="I23:J24"/>
+    <mergeCell ref="P23:Q24"/>
+    <mergeCell ref="R23:S24"/>
+    <mergeCell ref="M45:O48"/>
+    <mergeCell ref="B29:C32"/>
+    <mergeCell ref="B33:C35"/>
+    <mergeCell ref="D33:F35"/>
+    <mergeCell ref="B23:C24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="M12:O13"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="M14:O15"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="M18:O19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="M20:O21"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="M8:O9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="M10:O11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
     <mergeCell ref="D8:F10"/>
     <mergeCell ref="D6:F7"/>
     <mergeCell ref="G6:H7"/>
@@ -2739,79 +2824,6 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="D11:F13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="B16:C18"/>
-    <mergeCell ref="D16:F18"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="M8:O9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="M12:O13"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="M10:O11"/>
-    <mergeCell ref="M14:O15"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="M18:O19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="B29:C32"/>
-    <mergeCell ref="B33:C35"/>
-    <mergeCell ref="D33:F35"/>
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="G23:H24"/>
-    <mergeCell ref="I23:J24"/>
-    <mergeCell ref="P25:Q26"/>
-    <mergeCell ref="R25:S26"/>
-    <mergeCell ref="M47:O50"/>
-    <mergeCell ref="M51:O52"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="M30:O32"/>
-    <mergeCell ref="M33:O35"/>
-    <mergeCell ref="M36:O38"/>
-    <mergeCell ref="M39:O46"/>
-    <mergeCell ref="M25:O26"/>
-    <mergeCell ref="M27:O29"/>
-    <mergeCell ref="D25:F26"/>
-    <mergeCell ref="D27:F28"/>
-    <mergeCell ref="D29:F32"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M4:O5"/>
-    <mergeCell ref="D23:F24"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="P4:Q5"/>
-    <mergeCell ref="R4:S5"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="M6:O7"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="I18:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
mejoras caso de uso
</commit_message>
<xml_diff>
--- a/Documentacion/Parametros.xlsx
+++ b/Documentacion/Parametros.xlsx
@@ -646,182 +646,182 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1128,15 +1128,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="89" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
       <c r="K2" s="23"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
@@ -1177,38 +1177,38 @@
       <c r="AM3" s="3"/>
     </row>
     <row r="4" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="59" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59" t="s">
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59" t="s">
+      <c r="H4" s="86"/>
+      <c r="I4" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="59"/>
+      <c r="J4" s="86"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59" t="s">
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59" t="s">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="S4" s="59"/>
+      <c r="S4" s="86"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
@@ -1231,24 +1231,24 @@
       <c r="AM4" s="3"/>
     </row>
     <row r="5" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="76"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
@@ -1271,38 +1271,38 @@
       <c r="AM5" s="3"/>
     </row>
     <row r="6" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="94"/>
-      <c r="D6" s="53" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="53" t="s">
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="53" t="s">
+      <c r="H6" s="40"/>
+      <c r="I6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="54"/>
+      <c r="J6" s="40"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="55" t="s">
+      <c r="M6" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="55" t="s">
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="43" t="s">
+      <c r="Q6" s="68"/>
+      <c r="R6" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="S6" s="44"/>
+      <c r="S6" s="54"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -1325,30 +1325,30 @@
       <c r="AM6" s="3"/>
     </row>
     <row r="7" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="95"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="89"/>
-      <c r="I7" s="88" t="s">
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="89"/>
+      <c r="J7" s="46"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="49" t="s">
+      <c r="M7" s="69"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="45" t="s">
+      <c r="Q7" s="70"/>
+      <c r="R7" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="S7" s="41"/>
+      <c r="S7" s="72"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
@@ -1371,36 +1371,36 @@
       <c r="AM7" s="3"/>
     </row>
     <row r="8" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="95"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="53" t="s">
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="90"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="53" t="s">
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="54"/>
-      <c r="I8" s="53" t="s">
+      <c r="H8" s="40"/>
+      <c r="I8" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="55" t="s">
+      <c r="M8" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="55" t="s">
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="43" t="s">
+      <c r="Q8" s="68"/>
+      <c r="R8" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="S8" s="44"/>
+      <c r="S8" s="54"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
@@ -1423,30 +1423,30 @@
       <c r="AM8" s="3"/>
     </row>
     <row r="9" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="72" t="s">
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="73"/>
+      <c r="J9" s="43"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="57"/>
-      <c r="P9" s="49" t="s">
+      <c r="M9" s="69"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="45" t="s">
+      <c r="Q9" s="70"/>
+      <c r="R9" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="S9" s="41"/>
+      <c r="S9" s="72"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
@@ -1469,32 +1469,32 @@
       <c r="AM9" s="3"/>
     </row>
     <row r="10" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="95"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="72" t="s">
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="73"/>
+      <c r="J10" s="43"/>
       <c r="K10" s="24"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="42" t="s">
+      <c r="M10" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="N10" s="43"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="61" t="s">
+      <c r="N10" s="57"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="42" t="s">
+      <c r="Q10" s="87"/>
+      <c r="R10" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="S10" s="44"/>
+      <c r="S10" s="54"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
@@ -1517,34 +1517,34 @@
       <c r="AM10" s="3"/>
     </row>
     <row r="11" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="95"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="53" t="s">
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="90"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="53" t="s">
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="53" t="s">
+      <c r="H11" s="40"/>
+      <c r="I11" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="24"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="51" t="s">
+      <c r="M11" s="51"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="40" t="s">
+      <c r="Q11" s="88"/>
+      <c r="R11" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="S11" s="41"/>
+      <c r="S11" s="72"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
@@ -1567,34 +1567,34 @@
       <c r="AM11" s="3"/>
     </row>
     <row r="12" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="95"/>
-      <c r="C12" s="96"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="95" t="s">
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="96"/>
-      <c r="I12" s="72" t="s">
+      <c r="H12" s="50"/>
+      <c r="I12" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="73"/>
+      <c r="J12" s="43"/>
       <c r="K12" s="24"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="42" t="s">
+      <c r="M12" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="N12" s="43"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="52" t="s">
+      <c r="N12" s="57"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="42" t="s">
+      <c r="Q12" s="93"/>
+      <c r="R12" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="S12" s="44"/>
+      <c r="S12" s="54"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
@@ -1617,30 +1617,30 @@
       <c r="AM12" s="3"/>
     </row>
     <row r="13" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="95"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="88" t="s">
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="89"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="89"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="46"/>
       <c r="K13" s="24"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="51" t="s">
+      <c r="M13" s="51"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="40" t="s">
+      <c r="Q13" s="88"/>
+      <c r="R13" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S13" s="41"/>
+      <c r="S13" s="72"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
@@ -1663,36 +1663,36 @@
       <c r="AM13" s="3"/>
     </row>
     <row r="14" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="95"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="53" t="s">
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="90"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="53" t="s">
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="53" t="s">
+      <c r="H14" s="40"/>
+      <c r="I14" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="J14" s="54"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
-      <c r="M14" s="82" t="s">
+      <c r="M14" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="N14" s="83"/>
-      <c r="O14" s="84"/>
-      <c r="P14" s="55" t="s">
+      <c r="N14" s="62"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="43" t="s">
+      <c r="Q14" s="68"/>
+      <c r="R14" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="S14" s="44"/>
+      <c r="S14" s="54"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
@@ -1715,28 +1715,28 @@
       <c r="AM14" s="3"/>
     </row>
     <row r="15" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="95"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="73"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="43"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="49" t="s">
+      <c r="M15" s="64"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="69" t="s">
         <v>90</v>
       </c>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="45" t="s">
+      <c r="Q15" s="70"/>
+      <c r="R15" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="S15" s="41"/>
+      <c r="S15" s="72"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
@@ -1759,38 +1759,38 @@
       <c r="AM15" s="3"/>
     </row>
     <row r="16" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="42" t="s">
+      <c r="C16" s="54"/>
+      <c r="D16" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="42" t="s">
+      <c r="E16" s="57"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="44"/>
+      <c r="H16" s="54"/>
       <c r="I16" s="37" t="s">
         <v>62</v>
       </c>
       <c r="J16" s="35"/>
       <c r="K16" s="24"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="42" t="s">
+      <c r="M16" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="N16" s="43"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="80" t="s">
+      <c r="N16" s="57"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="42" t="s">
+      <c r="Q16" s="60"/>
+      <c r="R16" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="S16" s="44"/>
+      <c r="S16" s="54"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
@@ -1813,32 +1813,32 @@
       <c r="AM16" s="3"/>
     </row>
     <row r="17" spans="2:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="40" t="s">
+      <c r="B17" s="81"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="41"/>
+      <c r="H17" s="72"/>
       <c r="I17" s="36" t="s">
         <v>63</v>
       </c>
       <c r="J17" s="34"/>
       <c r="K17" s="24"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="46" t="s">
+      <c r="M17" s="51"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="46" t="s">
+      <c r="Q17" s="52"/>
+      <c r="R17" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="S17" s="48"/>
+      <c r="S17" s="52"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -1861,32 +1861,32 @@
       <c r="AM17" s="3"/>
     </row>
     <row r="18" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="40" t="s">
+      <c r="B18" s="81"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="72"/>
       <c r="K18" s="24"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="42" t="s">
+      <c r="M18" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="N18" s="43"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="42" t="s">
+      <c r="N18" s="57"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="42" t="s">
+      <c r="Q18" s="54"/>
+      <c r="R18" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="S18" s="44"/>
+      <c r="S18" s="54"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -1909,30 +1909,30 @@
       <c r="AM18" s="3"/>
     </row>
     <row r="19" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="46"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="38" t="s">
+      <c r="B19" s="51"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="95" t="s">
         <v>99</v>
       </c>
-      <c r="H19" s="39"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="52"/>
       <c r="K19" s="24"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="46" t="s">
+      <c r="M19" s="51"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="46" t="s">
+      <c r="Q19" s="52"/>
+      <c r="R19" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="S19" s="48"/>
+      <c r="S19" s="52"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
@@ -1966,19 +1966,19 @@
       <c r="J20" s="4"/>
       <c r="K20" s="24"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="55" t="s">
+      <c r="M20" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="55" t="s">
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="42" t="s">
+      <c r="Q20" s="68"/>
+      <c r="R20" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="S20" s="44"/>
+      <c r="S20" s="54"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
@@ -2012,17 +2012,17 @@
       <c r="J21" s="31"/>
       <c r="K21" s="4"/>
       <c r="L21" s="26"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="57"/>
-      <c r="P21" s="49" t="s">
+      <c r="M21" s="69"/>
+      <c r="N21" s="74"/>
+      <c r="O21" s="74"/>
+      <c r="P21" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="46" t="s">
+      <c r="Q21" s="70"/>
+      <c r="R21" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="S21" s="48"/>
+      <c r="S21" s="52"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
@@ -2082,38 +2082,38 @@
       <c r="AM22" s="3"/>
     </row>
     <row r="23" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="75"/>
-      <c r="D23" s="59" t="s">
+      <c r="C23" s="83"/>
+      <c r="D23" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59" t="s">
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59" t="s">
+      <c r="H23" s="86"/>
+      <c r="I23" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="59"/>
+      <c r="J23" s="86"/>
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
-      <c r="M23" s="59" t="s">
+      <c r="M23" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59" t="s">
+      <c r="N23" s="86"/>
+      <c r="O23" s="86"/>
+      <c r="P23" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59" t="s">
+      <c r="Q23" s="86"/>
+      <c r="R23" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="S23" s="59"/>
+      <c r="S23" s="86"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -2136,24 +2136,24 @@
       <c r="AM23" s="3"/>
     </row>
     <row r="24" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="76"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
       <c r="K24" s="4"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="59"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="86"/>
+      <c r="O24" s="86"/>
+      <c r="P24" s="86"/>
+      <c r="Q24" s="86"/>
+      <c r="R24" s="86"/>
+      <c r="S24" s="86"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -2176,15 +2176,15 @@
       <c r="AM24" s="3"/>
     </row>
     <row r="25" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="42" t="s">
+      <c r="C25" s="54"/>
+      <c r="D25" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="44"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="54"/>
       <c r="G25" s="5" t="s">
         <v>102</v>
       </c>
@@ -2194,11 +2194,11 @@
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="2"/>
-      <c r="M25" s="63" t="s">
+      <c r="M25" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="N25" s="64"/>
-      <c r="O25" s="65"/>
+      <c r="N25" s="76"/>
+      <c r="O25" s="77"/>
       <c r="P25" s="5" t="s">
         <v>103</v>
       </c>
@@ -2229,11 +2229,11 @@
       <c r="AM25" s="3"/>
     </row>
     <row r="26" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="46"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="48"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="7" t="s">
         <v>17</v>
       </c>
@@ -2243,17 +2243,17 @@
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="2"/>
-      <c r="M26" s="66"/>
-      <c r="N26" s="67"/>
-      <c r="O26" s="68"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="80"/>
       <c r="P26" s="21" t="s">
         <v>104</v>
       </c>
       <c r="Q26" s="11"/>
-      <c r="R26" s="78" t="s">
+      <c r="R26" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="S26" s="79"/>
+      <c r="S26" s="56"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -2276,15 +2276,15 @@
       <c r="AM26" s="3"/>
     </row>
     <row r="27" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="42" t="s">
+      <c r="C27" s="54"/>
+      <c r="D27" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="44"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="54"/>
       <c r="G27" s="5" t="s">
         <v>102</v>
       </c>
@@ -2294,9 +2294,9 @@
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="25"/>
-      <c r="M27" s="69"/>
-      <c r="N27" s="70"/>
-      <c r="O27" s="71"/>
+      <c r="M27" s="90"/>
+      <c r="N27" s="91"/>
+      <c r="O27" s="92"/>
       <c r="P27" s="7" t="s">
         <v>35</v>
       </c>
@@ -2305,11 +2305,11 @@
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="46"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="48"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="52"/>
       <c r="G28" s="7" t="s">
         <v>17</v>
       </c>
@@ -2319,11 +2319,11 @@
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="25"/>
-      <c r="M28" s="63" t="s">
+      <c r="M28" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="N28" s="64"/>
-      <c r="O28" s="65"/>
+      <c r="N28" s="76"/>
+      <c r="O28" s="77"/>
       <c r="P28" s="5" t="s">
         <v>105</v>
       </c>
@@ -2334,15 +2334,15 @@
       <c r="S28" s="6"/>
     </row>
     <row r="29" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="42" t="s">
+      <c r="C29" s="54"/>
+      <c r="D29" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="44"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="54"/>
       <c r="G29" s="10" t="s">
         <v>102</v>
       </c>
@@ -2352,9 +2352,9 @@
       </c>
       <c r="J29" s="14"/>
       <c r="K29" s="25"/>
-      <c r="M29" s="66"/>
-      <c r="N29" s="67"/>
-      <c r="O29" s="68"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="80"/>
       <c r="P29" s="21" t="s">
         <v>106</v>
       </c>
@@ -2365,11 +2365,11 @@
       <c r="S29" s="11"/>
     </row>
     <row r="30" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="41"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="72"/>
       <c r="G30" s="9" t="s">
         <v>107</v>
       </c>
@@ -2379,9 +2379,9 @@
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="25"/>
-      <c r="M30" s="69"/>
-      <c r="N30" s="70"/>
-      <c r="O30" s="71"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="92"/>
       <c r="P30" s="7" t="s">
         <v>38</v>
       </c>
@@ -2390,22 +2390,22 @@
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="41"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="72"/>
       <c r="G31" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="11"/>
       <c r="J31" s="16"/>
       <c r="K31" s="4"/>
-      <c r="M31" s="63" t="s">
+      <c r="M31" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="N31" s="64"/>
-      <c r="O31" s="65"/>
+      <c r="N31" s="76"/>
+      <c r="O31" s="77"/>
       <c r="P31" s="5" t="s">
         <v>108</v>
       </c>
@@ -2416,11 +2416,11 @@
       <c r="S31" s="6"/>
     </row>
     <row r="32" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="46"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="48"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="12" t="s">
         <v>24</v>
       </c>
@@ -2428,9 +2428,9 @@
       <c r="I32" s="17"/>
       <c r="J32" s="18"/>
       <c r="K32" s="4"/>
-      <c r="M32" s="66"/>
-      <c r="N32" s="67"/>
-      <c r="O32" s="68"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="79"/>
+      <c r="O32" s="80"/>
       <c r="P32" s="21" t="s">
         <v>109</v>
       </c>
@@ -2441,15 +2441,15 @@
       <c r="S32" s="11"/>
     </row>
     <row r="33" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="42" t="s">
+      <c r="C33" s="54"/>
+      <c r="D33" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="43"/>
-      <c r="F33" s="44"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="54"/>
       <c r="G33" s="10" t="s">
         <v>102</v>
       </c>
@@ -2459,9 +2459,9 @@
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="4"/>
-      <c r="M33" s="69"/>
-      <c r="N33" s="70"/>
-      <c r="O33" s="71"/>
+      <c r="M33" s="90"/>
+      <c r="N33" s="91"/>
+      <c r="O33" s="92"/>
       <c r="P33" s="7" t="s">
         <v>41</v>
       </c>
@@ -2470,11 +2470,11 @@
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="40"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="41"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="72"/>
       <c r="G34" s="21"/>
       <c r="H34" s="11"/>
       <c r="I34" s="28" t="s">
@@ -2482,11 +2482,11 @@
       </c>
       <c r="J34" s="11"/>
       <c r="K34" s="4"/>
-      <c r="M34" s="63" t="s">
+      <c r="M34" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="N34" s="64"/>
-      <c r="O34" s="65"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77"/>
       <c r="P34" s="5" t="s">
         <v>111</v>
       </c>
@@ -2497,20 +2497,20 @@
       <c r="S34" s="6"/>
     </row>
     <row r="35" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="46"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="48"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="52"/>
       <c r="G35" s="7"/>
       <c r="H35" s="8"/>
       <c r="I35" s="29" t="s">
         <v>59</v>
       </c>
       <c r="J35" s="8"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="67"/>
-      <c r="O35" s="68"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="80"/>
       <c r="P35" s="21" t="s">
         <v>113</v>
       </c>
@@ -2521,9 +2521,9 @@
       <c r="S35" s="11"/>
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M36" s="69"/>
-      <c r="N36" s="70"/>
-      <c r="O36" s="71"/>
+      <c r="M36" s="90"/>
+      <c r="N36" s="91"/>
+      <c r="O36" s="92"/>
       <c r="P36" s="7" t="s">
         <v>44</v>
       </c>
@@ -2532,11 +2532,11 @@
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M37" s="42" t="s">
+      <c r="M37" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="N37" s="43"/>
-      <c r="O37" s="44"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="54"/>
       <c r="P37" s="9" t="s">
         <v>92</v>
       </c>
@@ -2547,9 +2547,9 @@
       <c r="S37" s="6"/>
     </row>
     <row r="38" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M38" s="40"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
+      <c r="M38" s="81"/>
+      <c r="N38" s="71"/>
+      <c r="O38" s="71"/>
       <c r="P38" s="9" t="s">
         <v>47</v>
       </c>
@@ -2560,9 +2560,9 @@
       <c r="S38" s="11"/>
     </row>
     <row r="39" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M39" s="40"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
+      <c r="M39" s="81"/>
+      <c r="N39" s="71"/>
+      <c r="O39" s="71"/>
       <c r="P39" s="9" t="s">
         <v>46</v>
       </c>
@@ -2571,9 +2571,9 @@
       <c r="S39" s="11"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M40" s="40"/>
-      <c r="N40" s="45"/>
-      <c r="O40" s="41"/>
+      <c r="M40" s="81"/>
+      <c r="N40" s="71"/>
+      <c r="O40" s="72"/>
       <c r="P40" s="9" t="s">
         <v>103</v>
       </c>
@@ -2582,9 +2582,9 @@
       <c r="S40" s="11"/>
     </row>
     <row r="41" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M41" s="40"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="41"/>
+      <c r="M41" s="81"/>
+      <c r="N41" s="71"/>
+      <c r="O41" s="72"/>
       <c r="P41" s="9" t="s">
         <v>105</v>
       </c>
@@ -2592,9 +2592,9 @@
       <c r="S41" s="11"/>
     </row>
     <row r="42" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M42" s="40"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="41"/>
+      <c r="M42" s="81"/>
+      <c r="N42" s="71"/>
+      <c r="O42" s="72"/>
       <c r="P42" s="9" t="s">
         <v>108</v>
       </c>
@@ -2603,9 +2603,9 @@
       <c r="S42" s="11"/>
     </row>
     <row r="43" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M43" s="40"/>
-      <c r="N43" s="45"/>
-      <c r="O43" s="41"/>
+      <c r="M43" s="81"/>
+      <c r="N43" s="71"/>
+      <c r="O43" s="72"/>
       <c r="P43" s="9" t="s">
         <v>111</v>
       </c>
@@ -2614,9 +2614,9 @@
       <c r="S43" s="11"/>
     </row>
     <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M44" s="40"/>
-      <c r="N44" s="45"/>
-      <c r="O44" s="41"/>
+      <c r="M44" s="81"/>
+      <c r="N44" s="71"/>
+      <c r="O44" s="72"/>
       <c r="P44" s="9" t="s">
         <v>115</v>
       </c>
@@ -2625,11 +2625,11 @@
       <c r="S44" s="11"/>
     </row>
     <row r="45" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M45" s="63" t="s">
+      <c r="M45" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="N45" s="64"/>
-      <c r="O45" s="65"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="77"/>
       <c r="P45" s="10" t="s">
         <v>92</v>
       </c>
@@ -2640,9 +2640,9 @@
       <c r="S45" s="6"/>
     </row>
     <row r="46" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M46" s="66"/>
-      <c r="N46" s="67"/>
-      <c r="O46" s="68"/>
+      <c r="M46" s="78"/>
+      <c r="N46" s="79"/>
+      <c r="O46" s="80"/>
       <c r="P46" s="9" t="s">
         <v>103</v>
       </c>
@@ -2653,9 +2653,9 @@
       <c r="S46" s="11"/>
     </row>
     <row r="47" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M47" s="66"/>
-      <c r="N47" s="67"/>
-      <c r="O47" s="68"/>
+      <c r="M47" s="78"/>
+      <c r="N47" s="79"/>
+      <c r="O47" s="80"/>
       <c r="P47" s="9" t="s">
         <v>119</v>
       </c>
@@ -2666,9 +2666,9 @@
       <c r="S47" s="11"/>
     </row>
     <row r="48" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M48" s="66"/>
-      <c r="N48" s="67"/>
-      <c r="O48" s="68"/>
+      <c r="M48" s="78"/>
+      <c r="N48" s="79"/>
+      <c r="O48" s="80"/>
       <c r="P48" s="9" t="s">
         <v>121</v>
       </c>
@@ -2679,11 +2679,11 @@
       <c r="S48" s="11"/>
     </row>
     <row r="49" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M49" s="42" t="s">
+      <c r="M49" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="N49" s="43"/>
-      <c r="O49" s="44"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="54"/>
       <c r="P49" s="10" t="s">
         <v>102</v>
       </c>
@@ -2694,9 +2694,9 @@
       <c r="S49" s="6"/>
     </row>
     <row r="50" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M50" s="46"/>
-      <c r="N50" s="47"/>
-      <c r="O50" s="48"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="52"/>
       <c r="P50" s="7"/>
       <c r="Q50" s="8"/>
       <c r="R50" s="12" t="s">
@@ -2712,6 +2712,88 @@
     </row>
   </sheetData>
   <mergeCells count="98">
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="D16:F19"/>
+    <mergeCell ref="B16:C19"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M6:O7"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P4:Q5"/>
+    <mergeCell ref="R4:S5"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="M49:O50"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="M28:O30"/>
+    <mergeCell ref="M31:O33"/>
+    <mergeCell ref="M34:O36"/>
+    <mergeCell ref="M37:O44"/>
+    <mergeCell ref="M23:O24"/>
+    <mergeCell ref="M25:O27"/>
+    <mergeCell ref="D25:F26"/>
+    <mergeCell ref="D27:F28"/>
+    <mergeCell ref="D29:F32"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M4:O5"/>
+    <mergeCell ref="D23:F24"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="G23:H24"/>
+    <mergeCell ref="I23:J24"/>
+    <mergeCell ref="P23:Q24"/>
+    <mergeCell ref="R23:S24"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="M8:O9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="M10:O11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="M45:O48"/>
+    <mergeCell ref="B29:C32"/>
+    <mergeCell ref="B33:C35"/>
+    <mergeCell ref="D33:F35"/>
+    <mergeCell ref="B23:C24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="M12:O13"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="M14:O15"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="M18:O19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="M20:O21"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
     <mergeCell ref="D8:F10"/>
     <mergeCell ref="D6:F7"/>
     <mergeCell ref="G6:H7"/>
@@ -2728,88 +2810,6 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="D11:F13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="M12:O13"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="M14:O15"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="M18:O19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="M20:O21"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="M45:O48"/>
-    <mergeCell ref="B29:C32"/>
-    <mergeCell ref="B33:C35"/>
-    <mergeCell ref="D33:F35"/>
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="G23:H24"/>
-    <mergeCell ref="I23:J24"/>
-    <mergeCell ref="P23:Q24"/>
-    <mergeCell ref="R23:S24"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="M8:O9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="M10:O11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="M49:O50"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="M28:O30"/>
-    <mergeCell ref="M31:O33"/>
-    <mergeCell ref="M34:O36"/>
-    <mergeCell ref="M37:O44"/>
-    <mergeCell ref="M23:O24"/>
-    <mergeCell ref="M25:O27"/>
-    <mergeCell ref="D25:F26"/>
-    <mergeCell ref="D27:F28"/>
-    <mergeCell ref="D29:F32"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M4:O5"/>
-    <mergeCell ref="D23:F24"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="M6:O7"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P4:Q5"/>
-    <mergeCell ref="R4:S5"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="D16:F19"/>
-    <mergeCell ref="B16:C19"/>
-    <mergeCell ref="G16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modificsacion parametros seguridad(andres morales)
</commit_message>
<xml_diff>
--- a/Documentacion/Parametros.xlsx
+++ b/Documentacion/Parametros.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morales\Desktop\ProyectosGitHub\ProyectoAplicaciones\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8880"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="163">
   <si>
     <t>Cambio de Contraseña</t>
   </si>
@@ -317,15 +312,9 @@
     <t>Asignación de Opciones a Transacción</t>
   </si>
   <si>
-    <t>(1) Asignación de Opcioness Valida</t>
-  </si>
-  <si>
     <t>Código Privilegio</t>
   </si>
   <si>
-    <t>Opción</t>
-  </si>
-  <si>
     <t>(0) Error al Asignar Opciones</t>
   </si>
   <si>
@@ -402,13 +391,143 @@
   </si>
   <si>
     <t>Consulta de Producto Depreciasion</t>
+  </si>
+  <si>
+    <t>Log Operativo</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>(1) Registro Correcto</t>
+  </si>
+  <si>
+    <t>(0) Registro Incorrecto</t>
+  </si>
+  <si>
+    <t>Fecha Creacion</t>
+  </si>
+  <si>
+    <t>Codigo Usuario</t>
+  </si>
+  <si>
+    <t>Codigo del Proceso</t>
+  </si>
+  <si>
+    <t>Registro del Log Operativo por Proceso</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Codigo del Usuario</t>
+  </si>
+  <si>
+    <t>Asignación de Aplicación a Rol</t>
+  </si>
+  <si>
+    <t>(0) Error al Asignar Aplicación</t>
+  </si>
+  <si>
+    <t>(1) Asignación de Opciones Valida</t>
+  </si>
+  <si>
+    <t>(1) Asignación de Aplicaciones Valida</t>
+  </si>
+  <si>
+    <t>Registro Acciones</t>
+  </si>
+  <si>
+    <t>Código Accion</t>
+  </si>
+  <si>
+    <t>(1) Accion  Registrada</t>
+  </si>
+  <si>
+    <t>(0) Error al Registrar Accion</t>
+  </si>
+  <si>
+    <t>Asignación de Accion a Opcion</t>
+  </si>
+  <si>
+    <t>Accion</t>
+  </si>
+  <si>
+    <t>Opcion</t>
+  </si>
+  <si>
+    <t>(1) Asignación de Acciones Valida</t>
+  </si>
+  <si>
+    <t>(0) Error al Asignar Acción</t>
+  </si>
+  <si>
+    <t>Arreglo de Roles</t>
+  </si>
+  <si>
+    <t>Arreglo de Opciones</t>
+  </si>
+  <si>
+    <t>Arreglo deTransacciones</t>
+  </si>
+  <si>
+    <t>Control de Acceso al Sistema</t>
+  </si>
+  <si>
+    <t>Creacion de Usuario</t>
+  </si>
+  <si>
+    <t>Inventario</t>
+  </si>
+  <si>
+    <t>Cracion Producto</t>
+  </si>
+  <si>
+    <t>Toma Fisica</t>
+  </si>
+  <si>
+    <r>
+      <t>Movimiento Inv</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>entario</t>
+    </r>
+  </si>
+  <si>
+    <t>Creacion de empleado</t>
+  </si>
+  <si>
+    <t>Facturacion</t>
+  </si>
+  <si>
+    <t>Control Cierre Caja</t>
+  </si>
+  <si>
+    <t>Creacion de Factura</t>
+  </si>
+  <si>
+    <t>Control Anulacion de Factura</t>
+  </si>
+  <si>
+    <t>Registro del Log de Auditoria por Proceso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +553,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -568,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -654,52 +781,184 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -720,143 +979,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1130,7 +1336,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1138,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AM65"/>
+  <dimension ref="B2:AY65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:S21"/>
+    <sheetView tabSelected="1" topLeftCell="AO4" workbookViewId="0">
+      <selection activeCell="AU10" sqref="AU10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,22 +1362,25 @@
     <col min="12" max="12" width="8.7109375" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
     <col min="19" max="19" width="25.28515625" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="31" max="31" width="5.7109375" customWidth="1"/>
+    <col min="35" max="35" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D2" s="75" t="s">
+    <row r="2" spans="2:51" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D2" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
       <c r="K2" s="22"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21"/>
@@ -1181,8 +1390,11 @@
       <c r="Q2" s="21"/>
       <c r="R2" s="21"/>
       <c r="S2" s="21"/>
-    </row>
-    <row r="3" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="2:51" x14ac:dyDescent="0.25">
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -1208,482 +1420,631 @@
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AM3" s="3"/>
-    </row>
-    <row r="4" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+    </row>
+    <row r="4" spans="2:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="66" t="s">
+      <c r="C4" s="87"/>
+      <c r="D4" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66" t="s">
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66" t="s">
+      <c r="H4" s="69"/>
+      <c r="I4" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="66"/>
+      <c r="J4" s="69"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="66" t="s">
+      <c r="M4" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66" t="s">
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66" t="s">
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="S4" s="66"/>
+      <c r="S4" s="69"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
+      <c r="U4" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="V4" s="87"/>
+      <c r="W4" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="69"/>
+      <c r="Y4" s="69"/>
+      <c r="Z4" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA4" s="69"/>
+      <c r="AB4" s="126"/>
+      <c r="AC4" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD4" s="69"/>
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" s="69"/>
+      <c r="AH4" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI4" s="69"/>
       <c r="AJ4" s="3"/>
-      <c r="AK4" s="3"/>
-      <c r="AL4" s="3"/>
-      <c r="AM4" s="3"/>
-    </row>
-    <row r="5" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
+      <c r="AK4" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL4" s="87"/>
+      <c r="AM4" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN4" s="69"/>
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ4" s="69"/>
+      <c r="AS4" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT4" s="69"/>
+      <c r="AU4" s="69"/>
+      <c r="AV4" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW4" s="69"/>
+      <c r="AX4" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY4" s="69"/>
+    </row>
+    <row r="5" spans="2:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="88"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
       <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
+      <c r="U5" s="88"/>
+      <c r="V5" s="90"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="69"/>
+      <c r="Y5" s="69"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="69"/>
+      <c r="AB5" s="126"/>
+      <c r="AC5" s="69"/>
+      <c r="AD5" s="69"/>
+      <c r="AE5" s="69"/>
+      <c r="AF5" s="69"/>
+      <c r="AG5" s="69"/>
+      <c r="AH5" s="69"/>
+      <c r="AI5" s="69"/>
       <c r="AJ5" s="3"/>
-      <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
-    </row>
-    <row r="6" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="101" t="s">
+      <c r="AK5" s="88"/>
+      <c r="AL5" s="90"/>
+      <c r="AM5" s="69"/>
+      <c r="AN5" s="69"/>
+      <c r="AO5" s="69"/>
+      <c r="AP5" s="92"/>
+      <c r="AQ5" s="92"/>
+      <c r="AS5" s="69"/>
+      <c r="AT5" s="69"/>
+      <c r="AU5" s="69"/>
+      <c r="AV5" s="69"/>
+      <c r="AW5" s="69"/>
+      <c r="AX5" s="69"/>
+      <c r="AY5" s="69"/>
+    </row>
+    <row r="6" spans="2:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="67" t="s">
+      <c r="C6" s="94"/>
+      <c r="D6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="67" t="s">
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="67" t="s">
+      <c r="H6" s="39"/>
+      <c r="I6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="68"/>
+      <c r="J6" s="39"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="69" t="s">
+      <c r="M6" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
-      <c r="P6" s="69" t="s">
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="59" t="s">
+      <c r="Q6" s="56"/>
+      <c r="R6" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="42"/>
+      <c r="S6" s="14"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
+      <c r="U6" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="V6" s="48"/>
+      <c r="W6" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="X6" s="60"/>
+      <c r="Y6" s="61"/>
+      <c r="Z6" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA6" s="58"/>
       <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
+      <c r="AC6" s="114" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD6" s="115"/>
+      <c r="AE6" s="116"/>
+      <c r="AF6" s="110" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG6" s="109"/>
+      <c r="AH6" s="107" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI6" s="109"/>
       <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="3"/>
-    </row>
-    <row r="7" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="103"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="97"/>
-      <c r="I7" s="96" t="s">
+      <c r="AK6" s="127" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL6" s="128"/>
+      <c r="AM6" s="123" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN6" s="124"/>
+      <c r="AO6" s="124"/>
+      <c r="AP6" s="107" t="s">
+        <v>162</v>
+      </c>
+      <c r="AQ6" s="109"/>
+      <c r="AS6" s="114" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT6" s="115"/>
+      <c r="AU6" s="116"/>
+      <c r="AV6" s="107" t="s">
+        <v>162</v>
+      </c>
+      <c r="AW6" s="109"/>
+      <c r="AX6" s="107" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY6" s="109"/>
+    </row>
+    <row r="7" spans="2:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="95"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="97"/>
+      <c r="J7" s="45"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="62" t="s">
+      <c r="M7" s="54"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="60" t="s">
+      <c r="Q7" s="65"/>
+      <c r="R7" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="S7" s="44"/>
+      <c r="S7" s="18"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA7" s="104"/>
       <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
+      <c r="AC7" s="117"/>
+      <c r="AD7" s="118"/>
+      <c r="AE7" s="119"/>
+      <c r="AF7" s="110" t="s">
+        <v>129</v>
+      </c>
+      <c r="AG7" s="111"/>
+      <c r="AH7" s="110" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI7" s="111"/>
       <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
-    </row>
-    <row r="8" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="103"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="67" t="s">
+      <c r="AK7" s="129"/>
+      <c r="AL7" s="130"/>
+      <c r="AM7" s="54"/>
+      <c r="AN7" s="55"/>
+      <c r="AO7" s="55"/>
+      <c r="AP7" s="110" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ7" s="111"/>
+      <c r="AS7" s="117"/>
+      <c r="AT7" s="118"/>
+      <c r="AU7" s="119"/>
+      <c r="AV7" s="110" t="s">
+        <v>129</v>
+      </c>
+      <c r="AW7" s="111"/>
+      <c r="AX7" s="110" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY7" s="111"/>
+    </row>
+    <row r="8" spans="2:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="95"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="98"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="67" t="s">
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="68"/>
-      <c r="I8" s="67" t="s">
+      <c r="H8" s="39"/>
+      <c r="I8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="68"/>
+      <c r="J8" s="39"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="69" t="s">
+      <c r="M8" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
-      <c r="P8" s="69" t="s">
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="59" t="s">
+      <c r="Q8" s="56"/>
+      <c r="R8" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="S8" s="42"/>
+      <c r="S8" s="14"/>
       <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
+      <c r="U8" s="68"/>
+      <c r="V8" s="67"/>
+      <c r="W8" s="123" t="s">
+        <v>76</v>
+      </c>
+      <c r="X8" s="124"/>
+      <c r="Y8" s="125"/>
+      <c r="Z8" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA8" s="104"/>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
+      <c r="AC8" s="117"/>
+      <c r="AD8" s="118"/>
+      <c r="AE8" s="119"/>
+      <c r="AF8" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG8" s="111"/>
+      <c r="AH8" s="110"/>
+      <c r="AI8" s="111"/>
       <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-      <c r="AL8" s="3"/>
-      <c r="AM8" s="3"/>
-    </row>
-    <row r="9" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="103"/>
-      <c r="C9" s="104"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="91"/>
-      <c r="I9" s="90" t="s">
+      <c r="AK8" s="129"/>
+      <c r="AL8" s="130"/>
+      <c r="AM8" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="AN8" s="47"/>
+      <c r="AO8" s="47"/>
+      <c r="AP8" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="AQ8" s="111"/>
+      <c r="AS8" s="120"/>
+      <c r="AT8" s="121"/>
+      <c r="AU8" s="122"/>
+      <c r="AV8" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="AW8" s="113"/>
+      <c r="AX8" s="112"/>
+      <c r="AY8" s="113"/>
+    </row>
+    <row r="9" spans="2:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="95"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="91"/>
+      <c r="J9" s="42"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="71"/>
-      <c r="O9" s="71"/>
-      <c r="P9" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="60" t="s">
+      <c r="M9" s="54"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="S9" s="44"/>
+      <c r="S9" s="18"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="67"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="55"/>
+      <c r="Y9" s="65"/>
+      <c r="Z9" s="110"/>
+      <c r="AA9" s="111"/>
       <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
+      <c r="AC9" s="105"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="108"/>
+      <c r="AG9" s="108"/>
+      <c r="AH9" s="108"/>
+      <c r="AI9" s="108"/>
       <c r="AJ9" s="3"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="3"/>
-      <c r="AM9" s="3"/>
-    </row>
-    <row r="10" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="103"/>
-      <c r="C10" s="104"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="90" t="s">
+      <c r="AK9" s="129"/>
+      <c r="AL9" s="130"/>
+      <c r="AM9" s="49"/>
+      <c r="AN9" s="50"/>
+      <c r="AO9" s="50"/>
+      <c r="AP9" s="110"/>
+      <c r="AQ9" s="111"/>
+    </row>
+    <row r="10" spans="2:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="95"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="91"/>
+      <c r="J10" s="42"/>
       <c r="K10" s="23"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="59"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="74" t="s">
+      <c r="N10" s="47"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="41" t="s">
+      <c r="Q10" s="70"/>
+      <c r="R10" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="S10" s="42"/>
+      <c r="S10" s="14"/>
       <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="67"/>
+      <c r="W10" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="110"/>
+      <c r="AA10" s="111"/>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
+      <c r="AC10" s="106"/>
+      <c r="AD10" s="106"/>
+      <c r="AE10" s="106"/>
+      <c r="AF10" s="106"/>
+      <c r="AG10" s="106"/>
+      <c r="AH10" s="106"/>
+      <c r="AI10" s="106"/>
       <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="3"/>
-      <c r="AM10" s="3"/>
-    </row>
-    <row r="11" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="103"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="67" t="s">
+      <c r="AK10" s="129"/>
+      <c r="AL10" s="130"/>
+      <c r="AM10" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN10" s="47"/>
+      <c r="AO10" s="47"/>
+      <c r="AP10" s="110"/>
+      <c r="AQ10" s="111"/>
+    </row>
+    <row r="11" spans="2:51" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="95"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="98"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="67" t="s">
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="68"/>
-      <c r="I11" s="67" t="s">
+      <c r="H11" s="39"/>
+      <c r="I11" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="68"/>
+      <c r="J11" s="39"/>
       <c r="K11" s="23"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="64" t="s">
+      <c r="M11" s="49"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="43" t="s">
+      <c r="Q11" s="71"/>
+      <c r="R11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="S11" s="44"/>
+      <c r="S11" s="18"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
+      <c r="U11" s="68"/>
+      <c r="V11" s="67"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="110"/>
+      <c r="AA11" s="111"/>
       <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
+      <c r="AC11" s="106"/>
+      <c r="AD11" s="106"/>
+      <c r="AE11" s="106"/>
+      <c r="AF11" s="106"/>
+      <c r="AG11" s="106"/>
+      <c r="AH11" s="106"/>
+      <c r="AI11" s="106"/>
       <c r="AJ11" s="3"/>
-      <c r="AK11" s="3"/>
-      <c r="AL11" s="3"/>
-      <c r="AM11" s="3"/>
-    </row>
-    <row r="12" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="103"/>
-      <c r="C12" s="104"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="103" t="s">
+      <c r="AK11" s="129"/>
+      <c r="AL11" s="130"/>
+      <c r="AM11" s="49"/>
+      <c r="AN11" s="50"/>
+      <c r="AO11" s="50"/>
+      <c r="AP11" s="110"/>
+      <c r="AQ11" s="111"/>
+    </row>
+    <row r="12" spans="2:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="95"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="104"/>
-      <c r="I12" s="90" t="s">
+      <c r="H12" s="96"/>
+      <c r="I12" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="91"/>
+      <c r="J12" s="42"/>
       <c r="K12" s="23"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="41" t="s">
+      <c r="M12" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="N12" s="59"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="65" t="s">
+      <c r="N12" s="47"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="41" t="s">
+      <c r="Q12" s="91"/>
+      <c r="R12" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="S12" s="42"/>
+      <c r="S12" s="14"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
+      <c r="U12" s="68"/>
+      <c r="V12" s="67"/>
+      <c r="W12" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="110"/>
+      <c r="AA12" s="111"/>
       <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
-      <c r="AE12" s="3"/>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
+      <c r="AC12" s="106"/>
+      <c r="AD12" s="106"/>
+      <c r="AE12" s="106"/>
+      <c r="AF12" s="106"/>
+      <c r="AG12" s="106"/>
+      <c r="AH12" s="106"/>
+      <c r="AI12" s="106"/>
       <c r="AJ12" s="3"/>
-      <c r="AK12" s="3"/>
-      <c r="AL12" s="3"/>
-      <c r="AM12" s="3"/>
-    </row>
-    <row r="13" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="103"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="96" t="s">
+      <c r="AK12" s="129"/>
+      <c r="AL12" s="130"/>
+      <c r="AM12" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="47"/>
+      <c r="AO12" s="47"/>
+      <c r="AP12" s="110"/>
+      <c r="AQ12" s="111"/>
+    </row>
+    <row r="13" spans="2:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="95"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="97"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="97"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="45"/>
       <c r="K13" s="23"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="64" t="s">
+      <c r="M13" s="49"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="43" t="s">
+      <c r="Q13" s="71"/>
+      <c r="R13" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="S13" s="44"/>
+      <c r="S13" s="18"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
+      <c r="U13" s="49"/>
+      <c r="V13" s="51"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="51"/>
+      <c r="Z13" s="112"/>
+      <c r="AA13" s="113"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
@@ -1693,41 +2054,45 @@
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
       <c r="AJ13" s="3"/>
-      <c r="AK13" s="3"/>
-      <c r="AL13" s="3"/>
-      <c r="AM13" s="3"/>
-    </row>
-    <row r="14" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="103"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="67" t="s">
+      <c r="AK13" s="131"/>
+      <c r="AL13" s="132"/>
+      <c r="AM13" s="49"/>
+      <c r="AN13" s="50"/>
+      <c r="AO13" s="50"/>
+      <c r="AP13" s="110"/>
+      <c r="AQ13" s="111"/>
+    </row>
+    <row r="14" spans="2:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="95"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="98"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="67" t="s">
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="68"/>
-      <c r="I14" s="67" t="s">
+      <c r="H14" s="39"/>
+      <c r="I14" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="68"/>
+      <c r="J14" s="39"/>
       <c r="K14" s="29"/>
       <c r="L14" s="29"/>
-      <c r="M14" s="47" t="s">
+      <c r="M14" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="N14" s="48"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="69" t="s">
+      <c r="N14" s="60"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="Q14" s="72"/>
-      <c r="R14" s="59" t="s">
+      <c r="Q14" s="56"/>
+      <c r="R14" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="S14" s="42"/>
+      <c r="S14" s="14"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
@@ -1740,38 +2105,45 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
-      <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
-      <c r="AK14" s="3"/>
-      <c r="AL14" s="3"/>
-      <c r="AM14" s="3"/>
-    </row>
-    <row r="15" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="103"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="91"/>
+      <c r="AK14" s="127" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL14" s="128"/>
+      <c r="AM14" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN14" s="47"/>
+      <c r="AO14" s="47"/>
+      <c r="AP14" s="110"/>
+      <c r="AQ14" s="111"/>
+    </row>
+    <row r="15" spans="2:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="95"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="42"/>
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="60" t="s">
+      <c r="M15" s="62"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="S15" s="44"/>
+      <c r="S15" s="18"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
@@ -1789,43 +2161,47 @@
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
-      <c r="AK15" s="3"/>
-      <c r="AL15" s="3"/>
-      <c r="AM15" s="3"/>
-    </row>
-    <row r="16" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+      <c r="AK15" s="129"/>
+      <c r="AL15" s="130"/>
+      <c r="AM15" s="50"/>
+      <c r="AN15" s="50"/>
+      <c r="AO15" s="50"/>
+      <c r="AP15" s="110"/>
+      <c r="AQ15" s="111"/>
+    </row>
+    <row r="16" spans="2:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="41" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="47" t="s">
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="49"/>
+      <c r="H16" s="61"/>
       <c r="I16" s="36" t="s">
         <v>61</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="23"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="41" t="s">
+      <c r="M16" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="N16" s="59"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="94" t="s">
+      <c r="N16" s="47"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="Q16" s="95"/>
-      <c r="R16" s="41" t="s">
+      <c r="Q16" s="58"/>
+      <c r="R16" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="S16" s="42"/>
+      <c r="S16" s="14"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
@@ -1843,37 +2219,43 @@
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
-      <c r="AK16" s="3"/>
-      <c r="AL16" s="3"/>
-      <c r="AM16" s="3"/>
-    </row>
-    <row r="17" spans="2:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="43" t="s">
+      <c r="AK16" s="129"/>
+      <c r="AL16" s="130"/>
+      <c r="AM16" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="AN16" s="47"/>
+      <c r="AO16" s="47"/>
+      <c r="AP16" s="110"/>
+      <c r="AQ16" s="111"/>
+    </row>
+    <row r="17" spans="2:43" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="68"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="44"/>
+      <c r="H17" s="67"/>
       <c r="I17" s="35" t="s">
         <v>62</v>
       </c>
       <c r="J17" s="33"/>
       <c r="K17" s="23"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="45" t="s">
+      <c r="M17" s="49"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="45" t="s">
+      <c r="Q17" s="51"/>
+      <c r="R17" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="S17" s="46"/>
+      <c r="S17" s="18"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -1891,37 +2273,41 @@
       <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
       <c r="AJ17" s="3"/>
-      <c r="AK17" s="3"/>
-      <c r="AL17" s="3"/>
-      <c r="AM17" s="3"/>
-    </row>
-    <row r="18" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="43"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="43" t="s">
+      <c r="AK17" s="129"/>
+      <c r="AL17" s="130"/>
+      <c r="AM17" s="49"/>
+      <c r="AN17" s="50"/>
+      <c r="AO17" s="50"/>
+      <c r="AP17" s="110"/>
+      <c r="AQ17" s="111"/>
+    </row>
+    <row r="18" spans="2:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="68"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="44"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="44"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="67"/>
       <c r="K18" s="23"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="41" t="s">
+      <c r="M18" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="N18" s="59"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="41" t="s">
+      <c r="N18" s="47"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="S18" s="42"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="S18" s="14"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -1939,35 +2325,41 @@
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3"/>
-      <c r="AK18" s="3"/>
-      <c r="AL18" s="3"/>
-      <c r="AM18" s="3"/>
-    </row>
-    <row r="19" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="H19" s="58"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="46"/>
+      <c r="AK18" s="129"/>
+      <c r="AL18" s="130"/>
+      <c r="AM18" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN18" s="47"/>
+      <c r="AO18" s="47"/>
+      <c r="AP18" s="110"/>
+      <c r="AQ18" s="111"/>
+    </row>
+    <row r="19" spans="2:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="49"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="101" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="102"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="51"/>
       <c r="K19" s="23"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="S19" s="46"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="S19" s="18"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
@@ -1985,11 +2377,15 @@
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3"/>
-      <c r="AK19" s="3"/>
-      <c r="AL19" s="3"/>
-      <c r="AM19" s="3"/>
-    </row>
-    <row r="20" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AK19" s="131"/>
+      <c r="AL19" s="132"/>
+      <c r="AM19" s="49"/>
+      <c r="AN19" s="50"/>
+      <c r="AO19" s="50"/>
+      <c r="AP19" s="110"/>
+      <c r="AQ19" s="111"/>
+    </row>
+    <row r="20" spans="2:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
       <c r="D20" s="32"/>
@@ -2001,19 +2397,19 @@
       <c r="J20" s="4"/>
       <c r="K20" s="23"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="69" t="s">
+      <c r="M20" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="N20" s="70"/>
-      <c r="O20" s="70"/>
-      <c r="P20" s="69" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q20" s="72"/>
-      <c r="R20" s="41" t="s">
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="S20" s="42"/>
+      <c r="S20" s="14"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
@@ -2031,11 +2427,19 @@
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
       <c r="AJ20" s="3"/>
-      <c r="AK20" s="3"/>
-      <c r="AL20" s="3"/>
-      <c r="AM20" s="3"/>
-    </row>
-    <row r="21" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK20" s="127" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL20" s="128"/>
+      <c r="AM20" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN20" s="47"/>
+      <c r="AO20" s="47"/>
+      <c r="AP20" s="110"/>
+      <c r="AQ20" s="111"/>
+    </row>
+    <row r="21" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="30" t="s">
         <v>33</v>
       </c>
@@ -2047,17 +2451,17 @@
       <c r="J21" s="30"/>
       <c r="K21" s="4"/>
       <c r="L21" s="25"/>
-      <c r="M21" s="62"/>
-      <c r="N21" s="71"/>
-      <c r="O21" s="71"/>
-      <c r="P21" s="62" t="s">
+      <c r="M21" s="54"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="Q21" s="63"/>
-      <c r="R21" s="45" t="s">
+      <c r="Q21" s="65"/>
+      <c r="R21" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="S21" s="46"/>
+      <c r="S21" s="18"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
@@ -2075,11 +2479,15 @@
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
       <c r="AJ21" s="3"/>
-      <c r="AK21" s="3"/>
-      <c r="AL21" s="3"/>
-      <c r="AM21" s="3"/>
-    </row>
-    <row r="22" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK21" s="131"/>
+      <c r="AL21" s="132"/>
+      <c r="AM21" s="68"/>
+      <c r="AN21" s="66"/>
+      <c r="AO21" s="66"/>
+      <c r="AP21" s="110"/>
+      <c r="AQ21" s="111"/>
+    </row>
+    <row r="22" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2089,12 +2497,19 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="25"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
+      <c r="M22" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="N22" s="47"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="S22" s="14"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -2112,30 +2527,49 @@
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
       <c r="AJ22" s="3"/>
-      <c r="AK22" s="3"/>
-      <c r="AL22" s="3"/>
-      <c r="AM22" s="3"/>
-    </row>
-    <row r="23" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37" t="s">
+      <c r="AK22" s="127" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL22" s="133"/>
+      <c r="AM22" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="AN22" s="47"/>
+      <c r="AO22" s="47"/>
+      <c r="AP22" s="20"/>
+      <c r="AQ22" s="11"/>
+    </row>
+    <row r="23" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="66" t="s">
+      <c r="C23" s="87"/>
+      <c r="D23" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66" t="s">
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66" t="s">
+      <c r="H23" s="69"/>
+      <c r="I23" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="66"/>
+      <c r="J23" s="69"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="S23" s="18"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -2153,22 +2587,39 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
       <c r="AJ23" s="3"/>
-      <c r="AK23" s="3"/>
-      <c r="AL23" s="3"/>
-      <c r="AM23" s="3"/>
-    </row>
-    <row r="24" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
+      <c r="AK23" s="129"/>
+      <c r="AL23" s="134"/>
+      <c r="AM23" s="68"/>
+      <c r="AN23" s="66"/>
+      <c r="AO23" s="66"/>
+      <c r="AP23" s="20"/>
+      <c r="AQ23" s="11"/>
+    </row>
+    <row r="24" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="88"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
       <c r="K24" s="4"/>
       <c r="L24" s="19"/>
+      <c r="M24" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="N24" s="47"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="S24" s="14"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -2186,22 +2637,28 @@
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
       <c r="AJ24" s="3"/>
-      <c r="AK24" s="3"/>
-      <c r="AL24" s="3"/>
-      <c r="AM24" s="3"/>
-    </row>
-    <row r="25" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="41" t="s">
+      <c r="AK24" s="129"/>
+      <c r="AL24" s="134"/>
+      <c r="AM24" s="68" t="s">
+        <v>158</v>
+      </c>
+      <c r="AN24" s="66"/>
+      <c r="AO24" s="66"/>
+      <c r="AP24" s="20"/>
+      <c r="AQ24" s="11"/>
+    </row>
+    <row r="25" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="41" t="s">
+      <c r="C25" s="48"/>
+      <c r="D25" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="59"/>
-      <c r="F25" s="42"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
       <c r="G25" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="5" t="s">
@@ -2209,6 +2666,17 @@
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="2"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="S25" s="18"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -2226,16 +2694,20 @@
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
       <c r="AJ25" s="3"/>
-      <c r="AK25" s="3"/>
-      <c r="AL25" s="3"/>
-      <c r="AM25" s="3"/>
-    </row>
-    <row r="26" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="43"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="46"/>
+      <c r="AK25" s="129"/>
+      <c r="AL25" s="134"/>
+      <c r="AM25" s="68"/>
+      <c r="AN25" s="66"/>
+      <c r="AO25" s="66"/>
+      <c r="AP25" s="20"/>
+      <c r="AQ25" s="11"/>
+    </row>
+    <row r="26" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="68"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="51"/>
       <c r="G26" s="7" t="s">
         <v>17</v>
       </c>
@@ -2245,6 +2717,19 @@
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="2"/>
+      <c r="M26" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="N26" s="47"/>
+      <c r="O26" s="48"/>
+      <c r="P26" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q26" s="48"/>
+      <c r="R26" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="S26" s="14"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -2262,27 +2747,44 @@
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
       <c r="AJ26" s="3"/>
-      <c r="AK26" s="3"/>
-      <c r="AL26" s="3"/>
-      <c r="AM26" s="3"/>
-    </row>
-    <row r="27" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="43"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" s="48"/>
-      <c r="F27" s="49"/>
+      <c r="AK26" s="129"/>
+      <c r="AL26" s="134"/>
+      <c r="AM26" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN26" s="66"/>
+      <c r="AO26" s="66"/>
+      <c r="AP26" s="20"/>
+      <c r="AQ26" s="11"/>
+    </row>
+    <row r="27" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="68"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="60"/>
+      <c r="F27" s="61"/>
       <c r="G27" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J27" s="11"/>
       <c r="K27" s="2"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="S27" s="18"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
@@ -2300,16 +2802,20 @@
       <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
       <c r="AJ27" s="3"/>
-      <c r="AK27" s="3"/>
-      <c r="AL27" s="3"/>
-      <c r="AM27" s="3"/>
-    </row>
-    <row r="28" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="45"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="52"/>
+      <c r="AK27" s="131"/>
+      <c r="AL27" s="135"/>
+      <c r="AM27" s="49"/>
+      <c r="AN27" s="50"/>
+      <c r="AO27" s="50"/>
+      <c r="AP27" s="20"/>
+      <c r="AQ27" s="11"/>
+    </row>
+    <row r="28" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="49"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
       <c r="G28" s="20"/>
       <c r="H28" s="11"/>
       <c r="I28" s="20" t="s">
@@ -2334,22 +2840,30 @@
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
       <c r="AJ28" s="3"/>
-      <c r="AK28" s="3"/>
-      <c r="AL28" s="3"/>
-      <c r="AM28" s="3"/>
-    </row>
-    <row r="29" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="41" t="s">
+      <c r="AK28" s="127" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL28" s="128"/>
+      <c r="AM28" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="AN28" s="47"/>
+      <c r="AO28" s="47"/>
+      <c r="AP28" s="20"/>
+      <c r="AQ28" s="11"/>
+    </row>
+    <row r="29" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="41" t="s">
+      <c r="C29" s="48"/>
+      <c r="D29" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="59"/>
-      <c r="F29" s="42"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="48"/>
       <c r="G29" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="5" t="s">
@@ -2357,13 +2871,20 @@
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="24"/>
-    </row>
-    <row r="30" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="46"/>
+      <c r="AK29" s="131"/>
+      <c r="AL29" s="132"/>
+      <c r="AM29" s="49"/>
+      <c r="AN29" s="50"/>
+      <c r="AO29" s="50"/>
+      <c r="AP29" s="7"/>
+      <c r="AQ29" s="8"/>
+    </row>
+    <row r="30" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="49"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="51"/>
       <c r="G30" s="7" t="s">
         <v>17</v>
       </c>
@@ -2374,18 +2895,18 @@
       <c r="J30" s="8"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="41" t="s">
+    <row r="31" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="41" t="s">
+      <c r="C31" s="48"/>
+      <c r="D31" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="59"/>
-      <c r="F31" s="42"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="48"/>
       <c r="G31" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="13" t="s">
@@ -2394,14 +2915,14 @@
       <c r="J31" s="14"/>
       <c r="K31" s="24"/>
     </row>
-    <row r="32" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="43"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="44"/>
+    <row r="32" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="68"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="67"/>
       <c r="G32" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="15" t="s">
@@ -2411,11 +2932,11 @@
       <c r="K32" s="24"/>
     </row>
     <row r="33" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="44"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="67"/>
       <c r="G33" s="9" t="s">
         <v>17</v>
       </c>
@@ -2424,11 +2945,11 @@
       <c r="K33" s="4"/>
     </row>
     <row r="34" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="45"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="46"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="51"/>
       <c r="G34" s="12" t="s">
         <v>24</v>
       </c>
@@ -2438,17 +2959,17 @@
       <c r="K34" s="4"/>
     </row>
     <row r="35" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" s="48"/>
-      <c r="F35" s="49"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="60"/>
+      <c r="F35" s="61"/>
       <c r="G35" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="26" t="s">
@@ -2458,11 +2979,11 @@
       <c r="K35" s="4"/>
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="85"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="87"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="67"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="84"/>
       <c r="G36" s="20"/>
       <c r="H36" s="11"/>
       <c r="I36" s="27" t="s">
@@ -2472,11 +2993,11 @@
       <c r="K36" s="4"/>
     </row>
     <row r="37" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="45"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="52"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="64"/>
       <c r="G37" s="7"/>
       <c r="H37" s="8"/>
       <c r="I37" s="28" t="s">
@@ -2485,37 +3006,37 @@
       <c r="J37" s="8"/>
     </row>
     <row r="38" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M38" s="37" t="s">
+      <c r="M38" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="N38" s="88"/>
-      <c r="O38" s="38"/>
-      <c r="P38" s="37" t="s">
+      <c r="N38" s="86"/>
+      <c r="O38" s="87"/>
+      <c r="P38" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="Q38" s="38"/>
-      <c r="R38" s="37" t="s">
+      <c r="Q38" s="87"/>
+      <c r="R38" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="S38" s="38"/>
+      <c r="S38" s="87"/>
     </row>
     <row r="39" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M39" s="39"/>
+      <c r="M39" s="88"/>
       <c r="N39" s="89"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="39"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="39"/>
-      <c r="S39" s="40"/>
+      <c r="O39" s="90"/>
+      <c r="P39" s="88"/>
+      <c r="Q39" s="90"/>
+      <c r="R39" s="88"/>
+      <c r="S39" s="90"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M40" s="76" t="s">
+      <c r="M40" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="N40" s="77"/>
-      <c r="O40" s="78"/>
+      <c r="N40" s="74"/>
+      <c r="O40" s="75"/>
       <c r="P40" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q40" s="6"/>
       <c r="R40" s="5" t="s">
@@ -2524,22 +3045,22 @@
       <c r="S40" s="6"/>
     </row>
     <row r="41" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M41" s="79"/>
-      <c r="N41" s="80"/>
-      <c r="O41" s="81"/>
+      <c r="M41" s="76"/>
+      <c r="N41" s="77"/>
+      <c r="O41" s="78"/>
       <c r="P41" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q41" s="11"/>
-      <c r="R41" s="92" t="s">
+      <c r="R41" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="S41" s="93"/>
+      <c r="S41" s="104"/>
     </row>
     <row r="42" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M42" s="82"/>
-      <c r="N42" s="83"/>
-      <c r="O42" s="84"/>
+      <c r="M42" s="79"/>
+      <c r="N42" s="80"/>
+      <c r="O42" s="81"/>
       <c r="P42" s="7" t="s">
         <v>35</v>
       </c>
@@ -2548,13 +3069,13 @@
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M43" s="76" t="s">
+      <c r="M43" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="N43" s="77"/>
-      <c r="O43" s="78"/>
+      <c r="N43" s="74"/>
+      <c r="O43" s="75"/>
       <c r="P43" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q43" s="6"/>
       <c r="R43" s="5" t="s">
@@ -2563,11 +3084,11 @@
       <c r="S43" s="6"/>
     </row>
     <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M44" s="79"/>
-      <c r="N44" s="80"/>
-      <c r="O44" s="81"/>
+      <c r="M44" s="76"/>
+      <c r="N44" s="77"/>
+      <c r="O44" s="78"/>
       <c r="P44" s="20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q44" s="11"/>
       <c r="R44" s="20" t="s">
@@ -2576,9 +3097,9 @@
       <c r="S44" s="11"/>
     </row>
     <row r="45" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M45" s="82"/>
-      <c r="N45" s="83"/>
-      <c r="O45" s="84"/>
+      <c r="M45" s="79"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="81"/>
       <c r="P45" s="7" t="s">
         <v>38</v>
       </c>
@@ -2587,13 +3108,13 @@
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M46" s="76" t="s">
+      <c r="M46" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="N46" s="77"/>
-      <c r="O46" s="78"/>
+      <c r="N46" s="74"/>
+      <c r="O46" s="75"/>
       <c r="P46" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q46" s="6"/>
       <c r="R46" s="5" t="s">
@@ -2602,11 +3123,11 @@
       <c r="S46" s="6"/>
     </row>
     <row r="47" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M47" s="79"/>
-      <c r="N47" s="80"/>
-      <c r="O47" s="81"/>
+      <c r="M47" s="76"/>
+      <c r="N47" s="77"/>
+      <c r="O47" s="78"/>
       <c r="P47" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q47" s="11"/>
       <c r="R47" s="20" t="s">
@@ -2615,9 +3136,9 @@
       <c r="S47" s="11"/>
     </row>
     <row r="48" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M48" s="82"/>
-      <c r="N48" s="83"/>
-      <c r="O48" s="84"/>
+      <c r="M48" s="79"/>
+      <c r="N48" s="80"/>
+      <c r="O48" s="81"/>
       <c r="P48" s="7" t="s">
         <v>41</v>
       </c>
@@ -2626,37 +3147,37 @@
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M49" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="N49" s="77"/>
-      <c r="O49" s="78"/>
+      <c r="M49" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="N49" s="74"/>
+      <c r="O49" s="75"/>
       <c r="P49" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q49" s="6"/>
       <c r="R49" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S49" s="6"/>
     </row>
     <row r="50" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M50" s="79"/>
-      <c r="N50" s="80"/>
-      <c r="O50" s="81"/>
+      <c r="M50" s="76"/>
+      <c r="N50" s="77"/>
+      <c r="O50" s="78"/>
       <c r="P50" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q50" s="11"/>
       <c r="R50" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="S50" s="11"/>
     </row>
     <row r="51" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M51" s="82"/>
-      <c r="N51" s="83"/>
-      <c r="O51" s="84"/>
+      <c r="M51" s="79"/>
+      <c r="N51" s="80"/>
+      <c r="O51" s="81"/>
       <c r="P51" s="7" t="s">
         <v>44</v>
       </c>
@@ -2665,11 +3186,11 @@
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M52" s="47" t="s">
+      <c r="M52" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="N52" s="48"/>
-      <c r="O52" s="49"/>
+      <c r="N52" s="60"/>
+      <c r="O52" s="61"/>
       <c r="P52" s="9" t="s">
         <v>91</v>
       </c>
@@ -2680,9 +3201,9 @@
       <c r="S52" s="6"/>
     </row>
     <row r="53" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M53" s="85"/>
-      <c r="N53" s="86"/>
-      <c r="O53" s="87"/>
+      <c r="M53" s="82"/>
+      <c r="N53" s="83"/>
+      <c r="O53" s="84"/>
       <c r="P53" s="9" t="s">
         <v>47</v>
       </c>
@@ -2693,9 +3214,9 @@
       <c r="S53" s="11"/>
     </row>
     <row r="54" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M54" s="85"/>
-      <c r="N54" s="86"/>
-      <c r="O54" s="87"/>
+      <c r="M54" s="82"/>
+      <c r="N54" s="83"/>
+      <c r="O54" s="84"/>
       <c r="P54" s="9" t="s">
         <v>46</v>
       </c>
@@ -2704,132 +3225,132 @@
       <c r="S54" s="11"/>
     </row>
     <row r="55" spans="13:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M55" s="85"/>
-      <c r="N55" s="86"/>
-      <c r="O55" s="87"/>
+      <c r="M55" s="82"/>
+      <c r="N55" s="83"/>
+      <c r="O55" s="84"/>
       <c r="P55" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q55" s="11"/>
       <c r="R55" s="20"/>
       <c r="S55" s="11"/>
     </row>
     <row r="56" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M56" s="85"/>
-      <c r="N56" s="86"/>
-      <c r="O56" s="87"/>
+      <c r="M56" s="82"/>
+      <c r="N56" s="83"/>
+      <c r="O56" s="84"/>
       <c r="P56" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q56" s="11"/>
       <c r="S56" s="11"/>
     </row>
     <row r="57" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M57" s="85"/>
-      <c r="N57" s="86"/>
-      <c r="O57" s="87"/>
+      <c r="M57" s="82"/>
+      <c r="N57" s="83"/>
+      <c r="O57" s="84"/>
       <c r="P57" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q57" s="11"/>
       <c r="R57" s="20"/>
       <c r="S57" s="11"/>
     </row>
     <row r="58" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M58" s="85"/>
-      <c r="N58" s="86"/>
-      <c r="O58" s="87"/>
+      <c r="M58" s="82"/>
+      <c r="N58" s="83"/>
+      <c r="O58" s="84"/>
       <c r="P58" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q58" s="11"/>
       <c r="R58" s="20"/>
       <c r="S58" s="11"/>
     </row>
     <row r="59" spans="13:19" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M59" s="50"/>
-      <c r="N59" s="51"/>
-      <c r="O59" s="52"/>
-      <c r="P59" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q59" s="54"/>
+      <c r="M59" s="62"/>
+      <c r="N59" s="63"/>
+      <c r="O59" s="64"/>
+      <c r="P59" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q59" s="98"/>
       <c r="R59" s="20"/>
       <c r="S59" s="11"/>
     </row>
     <row r="60" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M60" s="76" t="s">
-        <v>115</v>
-      </c>
-      <c r="N60" s="77"/>
-      <c r="O60" s="78"/>
+      <c r="M60" s="73" t="s">
+        <v>113</v>
+      </c>
+      <c r="N60" s="74"/>
+      <c r="O60" s="75"/>
       <c r="P60" s="10" t="s">
         <v>91</v>
       </c>
       <c r="Q60" s="6"/>
       <c r="R60" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="S60" s="6"/>
     </row>
     <row r="61" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M61" s="79"/>
-      <c r="N61" s="80"/>
-      <c r="O61" s="81"/>
+      <c r="M61" s="76"/>
+      <c r="N61" s="77"/>
+      <c r="O61" s="78"/>
       <c r="P61" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q61" s="11"/>
       <c r="R61" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S61" s="11"/>
     </row>
     <row r="62" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M62" s="79"/>
-      <c r="N62" s="80"/>
-      <c r="O62" s="81"/>
+      <c r="M62" s="76"/>
+      <c r="N62" s="77"/>
+      <c r="O62" s="78"/>
       <c r="P62" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q62" s="11"/>
       <c r="R62" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="S62" s="11"/>
     </row>
     <row r="63" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M63" s="79"/>
-      <c r="N63" s="80"/>
-      <c r="O63" s="81"/>
+      <c r="M63" s="76"/>
+      <c r="N63" s="77"/>
+      <c r="O63" s="78"/>
       <c r="P63" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q63" s="11"/>
       <c r="R63" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="S63" s="11"/>
     </row>
     <row r="64" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M64" s="41" t="s">
+      <c r="M64" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="N64" s="59"/>
-      <c r="O64" s="42"/>
+      <c r="N64" s="47"/>
+      <c r="O64" s="48"/>
       <c r="P64" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q64" s="6"/>
-      <c r="R64" s="55" t="s">
+      <c r="R64" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="S64" s="56"/>
+      <c r="S64" s="100"/>
     </row>
     <row r="65" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M65" s="45"/>
-      <c r="N65" s="61"/>
-      <c r="O65" s="46"/>
+      <c r="M65" s="49"/>
+      <c r="N65" s="50"/>
+      <c r="O65" s="51"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="8"/>
       <c r="R65" s="12" t="s">
@@ -2838,60 +3359,77 @@
       <c r="S65" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="101">
-    <mergeCell ref="D11:F13"/>
-    <mergeCell ref="M18:O19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="M20:O21"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="M14:O15"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="M8:O9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="M10:O11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R4:S5"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="M64:O65"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="M43:O45"/>
-    <mergeCell ref="M46:O48"/>
-    <mergeCell ref="M49:O51"/>
-    <mergeCell ref="M52:O59"/>
-    <mergeCell ref="M38:O39"/>
-    <mergeCell ref="M40:O42"/>
-    <mergeCell ref="D25:F26"/>
-    <mergeCell ref="D29:F30"/>
-    <mergeCell ref="D31:F34"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M4:O5"/>
-    <mergeCell ref="D23:F24"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="G23:H24"/>
-    <mergeCell ref="I23:J24"/>
-    <mergeCell ref="R7:S7"/>
+  <mergeCells count="133">
+    <mergeCell ref="AM28:AO29"/>
+    <mergeCell ref="AK28:AL29"/>
+    <mergeCell ref="AS4:AU5"/>
+    <mergeCell ref="AV4:AW5"/>
+    <mergeCell ref="AX4:AY5"/>
+    <mergeCell ref="AS6:AU8"/>
+    <mergeCell ref="AM8:AO9"/>
+    <mergeCell ref="AM14:AO15"/>
+    <mergeCell ref="AM16:AO17"/>
+    <mergeCell ref="AM18:AO19"/>
+    <mergeCell ref="M26:O27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="AK4:AL5"/>
+    <mergeCell ref="AM4:AO5"/>
+    <mergeCell ref="AP4:AQ5"/>
+    <mergeCell ref="AK6:AL13"/>
+    <mergeCell ref="AM6:AO7"/>
+    <mergeCell ref="AM10:AO11"/>
+    <mergeCell ref="AM12:AO13"/>
+    <mergeCell ref="AK14:AL19"/>
+    <mergeCell ref="AM20:AO21"/>
+    <mergeCell ref="AK20:AL21"/>
+    <mergeCell ref="AM26:AO27"/>
+    <mergeCell ref="AK22:AL27"/>
+    <mergeCell ref="AM22:AO23"/>
+    <mergeCell ref="AM24:AO25"/>
+    <mergeCell ref="M22:O23"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="M24:O25"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="AH4:AI5"/>
+    <mergeCell ref="W8:Y9"/>
+    <mergeCell ref="W10:Y11"/>
+    <mergeCell ref="W12:Y13"/>
+    <mergeCell ref="U6:V13"/>
+    <mergeCell ref="AC6:AE8"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="Z4:AA5"/>
+    <mergeCell ref="U4:V5"/>
+    <mergeCell ref="W4:Y5"/>
+    <mergeCell ref="W6:Y7"/>
+    <mergeCell ref="AC4:AE5"/>
+    <mergeCell ref="AF4:AG5"/>
+    <mergeCell ref="R38:S39"/>
+    <mergeCell ref="P38:Q39"/>
+    <mergeCell ref="B25:C28"/>
+    <mergeCell ref="D27:F28"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="D16:F19"/>
+    <mergeCell ref="B16:C19"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="M60:O63"/>
+    <mergeCell ref="B31:C34"/>
+    <mergeCell ref="B35:C37"/>
+    <mergeCell ref="D35:F37"/>
+    <mergeCell ref="B23:C24"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="R41:S41"/>
+    <mergeCell ref="M16:O17"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="P13:Q13"/>
     <mergeCell ref="P12:Q12"/>
@@ -2916,30 +3454,45 @@
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="R38:S39"/>
-    <mergeCell ref="P38:Q39"/>
-    <mergeCell ref="B25:C28"/>
-    <mergeCell ref="D27:F28"/>
-    <mergeCell ref="P59:Q59"/>
-    <mergeCell ref="R64:S64"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="D16:F19"/>
-    <mergeCell ref="B16:C19"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="M60:O63"/>
-    <mergeCell ref="B31:C34"/>
-    <mergeCell ref="B35:C37"/>
-    <mergeCell ref="D35:F37"/>
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="R41:S41"/>
-    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="R4:S5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="M64:O65"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="M43:O45"/>
+    <mergeCell ref="M46:O48"/>
+    <mergeCell ref="M49:O51"/>
+    <mergeCell ref="M52:O59"/>
+    <mergeCell ref="M38:O39"/>
+    <mergeCell ref="M40:O42"/>
+    <mergeCell ref="D25:F26"/>
+    <mergeCell ref="D29:F30"/>
+    <mergeCell ref="D31:F34"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M4:O5"/>
+    <mergeCell ref="D23:F24"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="G23:H24"/>
+    <mergeCell ref="I23:J24"/>
+    <mergeCell ref="M8:O9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="M10:O11"/>
+    <mergeCell ref="D11:F13"/>
+    <mergeCell ref="M18:O19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="M20:O21"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="M14:O15"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>